<commit_message>
resetting 35% minimum dispatchable power
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_MIG-RE-NatLevUCs.xlsx
+++ b/SuppXLS/Scen_MIG-RE-NatLevUCs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda_models\IEMM_v60_10-1\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A49851EC-6947-4712-A7C6-89FC40056191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52156DAF-FDA6-4B92-84FF-E56FC2015168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3564" yWindow="-14184" windowWidth="17280" windowHeight="10044" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="6" r:id="rId1"/>
@@ -43633,8 +43633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="D1:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -43732,7 +43732,7 @@
         <v>1</v>
       </c>
       <c r="M9">
-        <v>-0.1</v>
+        <v>-0.35</v>
       </c>
       <c r="N9">
         <v>0</v>

</xml_diff>

<commit_message>
Adding the following files:   - infinite geological storage potentials   - limited technical life for the exosting power stock (except techs to be retrofitted)   - sensitivity case for dac costs   - calibration of the historical capacity
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_MIG-RE-NatLevUCs.xlsx
+++ b/SuppXLS/Scen_MIG-RE-NatLevUCs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda_models\IEMM_v60_10-1\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41393018-7FBB-4197-9F11-B488BFDA820B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{795D0903-CD05-4C39-8978-362A2350B85F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="6" r:id="rId1"/>
@@ -6654,8 +6654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C196069-B52A-2D4E-9CCF-B061AB993190}">
   <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6736,7 +6736,7 @@
   <dimension ref="B1:N206"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L4" sqref="L4:N234"/>
+      <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -43633,7 +43633,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="D1:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>

</xml_diff>